<commit_message>
final modification in bar chart
</commit_message>
<xml_diff>
--- a/mallikarjun/barchart.xlsx
+++ b/mallikarjun/barchart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BA7CBD-6D07-4CA6-80A4-5FADB53CB438}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32F9364-BD7B-4CDF-9FA4-C974A979FBEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,6 +95,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>North</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> America Sales for each Year</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -946,16 +976,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1249,7 +1279,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B12"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>